<commit_message>
Added default Schema, fixed courses not being printed for RankSchema output sheet
</commit_message>
<xml_diff>
--- a/demo/TestConfig.xlsx
+++ b/demo/TestConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Course Equivalents" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="199">
   <si>
     <t xml:space="preserve">CE3963</t>
   </si>
@@ -620,15 +620,6 @@
   </si>
   <si>
     <t xml:space="preserve">Senior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS1083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS2043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS3997</t>
   </si>
 </sst>
 </file>
@@ -723,12 +714,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -740,7 +731,7 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1739,10 +1730,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1778,22 +1769,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>